<commit_message>
I accounted for the occurence of a push in which event it counts it as a tie in the ATS record
</commit_message>
<xml_diff>
--- a/nfl_money_lines/nfl_money_lines.xlsx
+++ b/nfl_money_lines/nfl_money_lines.xlsx
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="G255" sqref="G255"/>
+    <sheetView tabSelected="1" topLeftCell="A251" workbookViewId="0">
+      <selection activeCell="F264" sqref="F264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7222,6 +7222,12 @@
       <c r="D261">
         <v>-220</v>
       </c>
+      <c r="E261">
+        <v>0</v>
+      </c>
+      <c r="F261">
+        <v>0</v>
+      </c>
       <c r="G261">
         <v>5</v>
       </c>
@@ -7242,6 +7248,12 @@
       <c r="D262">
         <v>-337</v>
       </c>
+      <c r="E262">
+        <v>0</v>
+      </c>
+      <c r="F262">
+        <v>0</v>
+      </c>
       <c r="G262">
         <v>7.5</v>
       </c>
@@ -7262,6 +7274,12 @@
       <c r="D263">
         <v>-197</v>
       </c>
+      <c r="E263">
+        <v>0</v>
+      </c>
+      <c r="F263">
+        <v>0</v>
+      </c>
       <c r="G263">
         <v>4</v>
       </c>
@@ -7281,6 +7299,12 @@
       </c>
       <c r="D264">
         <v>-379</v>
+      </c>
+      <c r="E264">
+        <v>0</v>
+      </c>
+      <c r="F264">
+        <v>0</v>
       </c>
       <c r="G264">
         <v>8</v>

</xml_diff>